<commit_message>
New York Times searching in nytimesSearch.py and JSON data stored in data2
</commit_message>
<xml_diff>
--- a/Newspapers.xlsx
+++ b/Newspapers.xlsx
@@ -232,9 +232,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="114">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -359,7 +362,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="114">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -472,6 +475,9 @@
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -562,7 +568,7 @@
     </tableColumn>
     <tableColumn id="6" name="URL" totalsRowDxfId="1"/>
     <tableColumn id="7" name="JSON" dataDxfId="7" totalsRowDxfId="0">
-      <calculatedColumnFormula>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</calculatedColumnFormula>
+      <calculatedColumnFormula>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -893,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -980,8 +986,8 @@
         <v>6</v>
       </c>
       <c r="G4" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s1 = {'publication':'SF Gate','date': 20121003,'url':'http://www.sfgate.com/politics/article/Romney-Obama-square-off-in-polite-debate-3917947.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s1 = {'publication':'SF Gate','date': 20121003,'url':'http://www.sfgate.com/politics/article/Romney-Obama-square-off-in-polite-debate-3917947.php',debate:'1'};</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1005,8 +1011,8 @@
         <v>7</v>
       </c>
       <c r="G5" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s2 = {'publication':'SF Gate','date': 20121003,'url':'http://www.sfgate.com/news/article/Aggressive-Romney-spars-with-Obama-in-first-debate-3914354.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s2 = {'publication':'SF Gate','date': 20121003,'url':'http://www.sfgate.com/news/article/Aggressive-Romney-spars-with-Obama-in-first-debate-3914354.php',debate:'1'};</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1030,8 +1036,8 @@
         <v>8</v>
       </c>
       <c r="G6" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s3 = {'publication':'SF Gate','date': 20121003,'url':'http://www.sfgate.com/science/article/Candidates-ignore-climate-change-debate-3914294.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s3 = {'publication':'SF Gate','date': 20121003,'url':'http://www.sfgate.com/science/article/Candidates-ignore-climate-change-debate-3914294.php',debate:'1'};</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1055,8 +1061,8 @@
         <v>9</v>
       </c>
       <c r="G7" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s4 = {'publication':'SF Gate','date': 20121004,'url':'http://www.sfgate.com/news/article/Romney-Victory-is-in-sight-after-first-debate-3918050.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s4 = {'publication':'SF Gate','date': 20121004,'url':'http://www.sfgate.com/news/article/Romney-Victory-is-in-sight-after-first-debate-3918050.php',debate:'1'};</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1080,8 +1086,8 @@
         <v>10</v>
       </c>
       <c r="G8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s5 = {'publication':'SF Gate','date': 20121004,'url':'http://www.sfgate.com/entertainment/article/Tough-reviews-for-Jim-Lehrer-as-debate-moderator-3917905.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s5 = {'publication':'SF Gate','date': 20121004,'url':'http://www.sfgate.com/entertainment/article/Tough-reviews-for-Jim-Lehrer-as-debate-moderator-3917905.php',debate:'1'};</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1105,8 +1111,8 @@
         <v>11</v>
       </c>
       <c r="G9" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s6 = {'publication':'SF Gate','date': 20121005,'url':'http://www.sfgate.com/news/article/Obama-Romney-mix-humor-into-rallies-fundraisers-3922743.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s6 = {'publication':'SF Gate','date': 20121005,'url':'http://www.sfgate.com/news/article/Obama-Romney-mix-humor-into-rallies-fundraisers-3922743.php',debate:'1'};</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1130,8 +1136,8 @@
         <v>12</v>
       </c>
       <c r="G10" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s7 = {'publication':'SF Gate','date': 20121005,'url':'http://www.sfgate.com/business/article/Romney-s-Medicare-plan-raises-cost-questions-3921172.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s7 = {'publication':'SF Gate','date': 20121005,'url':'http://www.sfgate.com/business/article/Romney-s-Medicare-plan-raises-cost-questions-3921172.php',debate:'1'};</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1155,8 +1161,8 @@
         <v>5</v>
       </c>
       <c r="G11" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s8 = {'publication':'SF Gate','date': 20121006,'url':'http://www.sfgate.com/business/prweb/article/Absolute-Rights-Online-Article-Prepares-for-3924605.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s8 = {'publication':'SF Gate','date': 20121006,'url':'http://www.sfgate.com/business/prweb/article/Absolute-Rights-Online-Article-Prepares-for-3924605.php',debate:'1'};</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1180,8 +1186,8 @@
         <v>13</v>
       </c>
       <c r="G12" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s9 = {'publication':'SF Gate','date': 20121007,'url':'http://www.sfgate.com/opinion/openforum/article/Nuns-on-the-Bus-role-in-campaign-3926797.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s9 = {'publication':'SF Gate','date': 20121007,'url':'http://www.sfgate.com/opinion/openforum/article/Nuns-on-the-Bus-role-in-campaign-3926797.php',debate:'1'};</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1205,8 +1211,8 @@
         <v>14</v>
       </c>
       <c r="G13" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s10 = {'publication':'SF Gate','date': 20121007,'url':'http://www.sfgate.com/news/article/Post-debate-poll-shows-tightening-race-in-Colorado-3926464.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s10 = {'publication':'SF Gate','date': 20121007,'url':'http://www.sfgate.com/news/article/Post-debate-poll-shows-tightening-race-in-Colorado-3926464.php',debate:'1'};</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1230,8 +1236,8 @@
         <v>18</v>
       </c>
       <c r="G14" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s11 = {'publication':'SF Gate','date': 20121008,'url':'http://www.sfgate.com/news/article/Obama-Romney-use-humor-into-connect-with-voters-3924357.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s11 = {'publication':'SF Gate','date': 20121008,'url':'http://www.sfgate.com/news/article/Obama-Romney-use-humor-into-connect-with-voters-3924357.php',debate:'1'};</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1255,8 +1261,8 @@
         <v>17</v>
       </c>
       <c r="G15" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s12 = {'publication':'SF Gate','date': 20121009,'url':'http://blog.sfgate.com/nov05election/category/presidential-debates/'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s12 = {'publication':'SF Gate','date': 20121009,'url':'http://blog.sfgate.com/nov05election/category/presidential-debates/',debate:'1'};</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1280,8 +1286,8 @@
         <v>19</v>
       </c>
       <c r="G16" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s13 = {'publication':'SF Gate','date': 20121010,'url':'http://www.sfgate.com/business/bloomberg/article/Romney-Fights-in-Ohio-With-Fresh-Confidence-From-3933258.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s13 = {'publication':'SF Gate','date': 20121010,'url':'http://www.sfgate.com/business/bloomberg/article/Romney-Fights-in-Ohio-With-Fresh-Confidence-From-3933258.php',debate:'1'};</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1305,8 +1311,8 @@
         <v>20</v>
       </c>
       <c r="G17" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s14 = {'publication':'SF Gate','date': 20121011,'url':'http://www.sfgate.com/business/bloomberg/article/Romney-Win-to-Help-Banks-Hurt-Clean-Energy-3940111.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s14 = {'publication':'SF Gate','date': 20121011,'url':'http://www.sfgate.com/business/bloomberg/article/Romney-Win-to-Help-Banks-Hurt-Clean-Energy-3940111.php',debate:'1'};</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1330,8 +1336,8 @@
         <v>21</v>
       </c>
       <c r="G18" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s15 = {'publication':'SF Gate','date': 20121011,'url':'http://www.sfgate.com/business/bloomberg/article/Romney-Closes-Gap-With-Obama-in-Five-Swing-State-3940677.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s15 = {'publication':'SF Gate','date': 20121011,'url':'http://www.sfgate.com/business/bloomberg/article/Romney-Closes-Gap-With-Obama-in-Five-Swing-State-3940677.php',debate:'1'};</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1355,8 +1361,8 @@
         <v>22</v>
       </c>
       <c r="G19" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s16 = {'publication':'SF Gate','date': 20121012,'url':'http://www.sfgate.com/news/article/THE-RACE-Obama-Romney-2nd-debate-next-up-in-race-3942706.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s16 = {'publication':'SF Gate','date': 20121012,'url':'http://www.sfgate.com/news/article/THE-RACE-Obama-Romney-2nd-debate-next-up-in-race-3942706.php',debate:'2'};</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1380,8 +1386,8 @@
         <v>23</v>
       </c>
       <c r="G20" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s17 = {'publication':'SF Gate','date': 20121012,'url':'http://www.sfgate.com/news/article/Diminished-GOP-brand-heightens-Romney-s-challenge-3930796.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s17 = {'publication':'SF Gate','date': 20121012,'url':'http://www.sfgate.com/news/article/Diminished-GOP-brand-heightens-Romney-s-challenge-3930796.php',debate:'1'};</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1405,8 +1411,8 @@
         <v>24</v>
       </c>
       <c r="G21" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s18 = {'publication':'SF Gate','date': 20121013,'url':'http://www.sfgate.com/news/article/Obama-on-debate-with-Romney-I-had-a-bad-night-3934254.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s18 = {'publication':'SF Gate','date': 20121013,'url':'http://www.sfgate.com/news/article/Obama-on-debate-with-Romney-I-had-a-bad-night-3934254.php',debate:'1'};</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1430,8 +1436,8 @@
         <v>25</v>
       </c>
       <c r="G22" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s19 = {'publication':'SF Gate','date': 20121014,'url':'http://www.sfgate.com/politics/article/Obama-Romney-campaigns-prep-for-debate-3948527.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s19 = {'publication':'SF Gate','date': 20121014,'url':'http://www.sfgate.com/politics/article/Obama-Romney-campaigns-prep-for-debate-3948527.php',debate:'2'};</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1455,8 +1461,8 @@
         <v>26</v>
       </c>
       <c r="G23" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s20 = {'publication':'SF Gate','date': 20121015,'url':'http://www.sfgate.com/politics/article/Goals-for-Obama-Romney-in-next-debate-3951478.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s20 = {'publication':'SF Gate','date': 20121015,'url':'http://www.sfgate.com/politics/article/Goals-for-Obama-Romney-in-next-debate-3951478.php',debate:'2'};</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1480,8 +1486,8 @@
         <v>27</v>
       </c>
       <c r="G24" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s21 = {'publication':'SF Gate','date': 20121015,'url':'http://www.sfgate.com/politics/joegarofoli/article/Pivots-key-to-Romney-Obama-debate-3951481.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s21 = {'publication':'SF Gate','date': 20121015,'url':'http://www.sfgate.com/politics/joegarofoli/article/Pivots-key-to-Romney-Obama-debate-3951481.php',debate:'2'};</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1505,8 +1511,8 @@
         <v>28</v>
       </c>
       <c r="G25" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s22 = {'publication':'SF Gate','date': 20121016,'url':'http://www.sfgate.com/politics/article/Obama-Romney-come-out-fighting-in-N-Y-3954933.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s22 = {'publication':'SF Gate','date': 20121016,'url':'http://www.sfgate.com/politics/article/Obama-Romney-come-out-fighting-in-N-Y-3954933.php',debate:'2'};</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1530,8 +1536,8 @@
         <v>29</v>
       </c>
       <c r="G26" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s23 = {'publication':'SF Gate','date': 20121016,'url':'http://www.sfgate.com/politics/joegarofoli/article/GOP-lacks-incentive-to-provide-details-3951474.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s23 = {'publication':'SF Gate','date': 20121016,'url':'http://www.sfgate.com/politics/joegarofoli/article/GOP-lacks-incentive-to-provide-details-3951474.php',debate:'2'};</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1555,8 +1561,8 @@
         <v>33</v>
       </c>
       <c r="G27" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s24 = {'publication':'SF Gate','date': 20121016,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Says-Romney-Words-Aren-t-True-as-3954437.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s24 = {'publication':'SF Gate','date': 20121016,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Says-Romney-Words-Aren-t-True-as-3954437.php',debate:'2'};</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1580,8 +1586,8 @@
         <v>34</v>
       </c>
       <c r="G28" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s25 = {'publication':'SF Gate','date': 20121017,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Won-Second-Presidential-Debate-46-Percent-3955094.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s25 = {'publication':'SF Gate','date': 20121017,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Won-Second-Presidential-Debate-46-Percent-3955094.php',debate:'2'};</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1605,8 +1611,8 @@
         <v>35</v>
       </c>
       <c r="G29" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s26 = {'publication':'SF Gate','date': 20121017,'url':'http://www.sfgate.com/politics/article/Obama-Romney-get-testy-in-2nd-debate-3954943.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s26 = {'publication':'SF Gate','date': 20121017,'url':'http://www.sfgate.com/politics/article/Obama-Romney-get-testy-in-2nd-debate-3954943.php',debate:'2'};</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1630,8 +1636,8 @@
         <v>36</v>
       </c>
       <c r="G30" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s27 = {'publication':'SF Gate','date': 20121018,'url':'http://www.sfgate.com/politics/article/Obama-rebuffs-Romney-on-consulate-attack-3962651.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s27 = {'publication':'SF Gate','date': 20121018,'url':'http://www.sfgate.com/politics/article/Obama-rebuffs-Romney-on-consulate-attack-3962651.php',debate:'2'};</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1655,8 +1661,8 @@
         <v>37</v>
       </c>
       <c r="G31" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s28 = {'publication':'SF Gate','date': 20121018,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Won-Second-Presidential-Debate-CNN-Voter-3957640.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s28 = {'publication':'SF Gate','date': 20121018,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Won-Second-Presidential-Debate-CNN-Voter-3957640.php',debate:'2'};</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1680,8 +1686,8 @@
         <v>38</v>
       </c>
       <c r="G32" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s29 = {'publication':'SF Gate','date': 20121018,'url':'http://www.sfgate.com/politics/article/Binders-full-of-women-sweeps-social-media-3957833.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s29 = {'publication':'SF Gate','date': 20121018,'url':'http://www.sfgate.com/politics/article/Binders-full-of-women-sweeps-social-media-3957833.php',debate:'2'};</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1705,8 +1711,8 @@
         <v>39</v>
       </c>
       <c r="G33" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s30 = {'publication':'SF Gate','date': 20121019,'url':'http://www.sfgate.com/news/politics/article/Obama-accuses-Romney-of-suffering-from-Romnesia-3964216.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s30 = {'publication':'SF Gate','date': 20121019,'url':'http://www.sfgate.com/news/politics/article/Obama-accuses-Romney-of-suffering-from-Romnesia-3964216.php',debate:'2'};</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1730,8 +1736,8 @@
         <v>40</v>
       </c>
       <c r="G34" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s31 = {'publication':'SF Gate','date': 20121019,'url':'http://www.sfgate.com/news/politics/article/Analysis-In-blistering-form-Obama-rebounds-3951562.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s31 = {'publication':'SF Gate','date': 20121019,'url':'http://www.sfgate.com/news/politics/article/Analysis-In-blistering-form-Obama-rebounds-3951562.php',debate:'2'};</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1755,8 +1761,8 @@
         <v>41</v>
       </c>
       <c r="G35" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s32 = {'publication':'SF Gate','date': 20121020,'url':'http://www.sfgate.com/news/politics/article/Romney-ups-criticism-of-Obama-s-second-term-plans-3966267.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s32 = {'publication':'SF Gate','date': 20121020,'url':'http://www.sfgate.com/news/politics/article/Romney-ups-criticism-of-Obama-s-second-term-plans-3966267.php',debate:'2'};</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1780,8 +1786,8 @@
         <v>42</v>
       </c>
       <c r="G36" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s33 = {'publication':'SF Gate','date': 20121020,'url':'http://www.sfgate.com/politics/article/Romney-rips-Obama-over-plans-for-future-3967713.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s33 = {'publication':'SF Gate','date': 20121020,'url':'http://www.sfgate.com/politics/article/Romney-rips-Obama-over-plans-for-future-3967713.php',debate:'2'};</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1805,8 +1811,8 @@
         <v>43</v>
       </c>
       <c r="G37" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s34 = {'publication':'SF Gate','date': 20121021,'url':'http://www.sfgate.com/news/politics/article/Stand-up-Obama-and-Romney-draw-laughs-at-dinner-3962840.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s34 = {'publication':'SF Gate','date': 20121021,'url':'http://www.sfgate.com/news/politics/article/Stand-up-Obama-and-Romney-draw-laughs-at-dinner-3962840.php',debate:'2'};</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1830,8 +1836,8 @@
         <v>44</v>
       </c>
       <c r="G38" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s35 = {'publication':'SF Gate','date': 20121021,'url':'http://www.sfgate.com/news/politics/article/Obama-Romney-allies-square-off-on-foreign-policy-3968460.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s35 = {'publication':'SF Gate','date': 20121021,'url':'http://www.sfgate.com/news/politics/article/Obama-Romney-allies-square-off-on-foreign-policy-3968460.php',debate:'3'};</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1855,8 +1861,8 @@
         <v>45</v>
       </c>
       <c r="G39" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s36 = {'publication':'SF Gate','date': 20121022,'url':'http://www.sfgate.com/opinion/saunders/article/Obama-vs-Romney-the-peacenik-3972657.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s36 = {'publication':'SF Gate','date': 20121022,'url':'http://www.sfgate.com/opinion/saunders/article/Obama-vs-Romney-the-peacenik-3972657.php',debate:'3'};</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1880,8 +1886,8 @@
         <v>46</v>
       </c>
       <c r="G40" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s37 = {'publication':'SF Gate','date': 20121022,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Trades-Foreign-Policy-Attacks-With-Romney-3972616.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s37 = {'publication':'SF Gate','date': 20121022,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Trades-Foreign-Policy-Attacks-With-Romney-3972616.php',debate:'3'};</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1905,8 +1911,8 @@
         <v>47</v>
       </c>
       <c r="G41" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s38 = {'publication':'SF Gate','date': 20121023,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Won-Final-Presidential-Debate-48-Percent-3972907.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s38 = {'publication':'SF Gate','date': 20121023,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Won-Final-Presidential-Debate-48-Percent-3972907.php',debate:'3'};</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1930,8 +1936,8 @@
         <v>48</v>
       </c>
       <c r="G42" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s39 = {'publication':'SF Gate','date': 20121023,'url':'http://www.sfgate.com/politics/article/Obama-feisty-Romney-subdued-in-debate-3972825.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s39 = {'publication':'SF Gate','date': 20121023,'url':'http://www.sfgate.com/politics/article/Obama-feisty-Romney-subdued-in-debate-3972825.php',debate:'3'};</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1955,8 +1961,8 @@
         <v>49</v>
       </c>
       <c r="G43" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s40 = {'publication':'SF Gate','date': 20121024,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Romney-Race-Has-Both-Arguing-Plausible-Path-3976211.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s40 = {'publication':'SF Gate','date': 20121024,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Romney-Race-Has-Both-Arguing-Plausible-Path-3976211.php',debate:'3'};</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1980,8 +1986,8 @@
         <v>50</v>
       </c>
       <c r="G44" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s41 = {'publication':'SF Gate','date': 20121025,'url':'http://www.sfgate.com/news/science/article/Guns-climate-gays-missing-in-presidential-race-3979757.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s41 = {'publication':'SF Gate','date': 20121025,'url':'http://www.sfgate.com/news/science/article/Guns-climate-gays-missing-in-presidential-race-3979757.php',debate:'3'};</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2005,8 +2011,8 @@
         <v>51</v>
       </c>
       <c r="G45" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s42 = {'publication':'SF Gate','date': 20121026,'url':'http://www.sfgate.com/opinion/editorials/article/Chronicle-recommends-Re-elect-Obama-3985242.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s42 = {'publication':'SF Gate','date': 20121026,'url':'http://www.sfgate.com/opinion/editorials/article/Chronicle-recommends-Re-elect-Obama-3985242.php',debate:'3'};</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2030,8 +2036,8 @@
         <v>52</v>
       </c>
       <c r="G46" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s43 = {'publication':'SF Gate','date': 20121027,'url':'http://www.sfgate.com/news/politics/article/Obama-hits-Romney-on-taxes-Massachusetts-record-3986813.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s43 = {'publication':'SF Gate','date': 20121027,'url':'http://www.sfgate.com/news/politics/article/Obama-hits-Romney-on-taxes-Massachusetts-record-3986813.php',debate:'3'};</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2055,8 +2061,8 @@
         <v>53</v>
       </c>
       <c r="G47" s="8" t="str">
-        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"'};")</f>
-        <v>var s44 = {'publication':'SF Gate','date': 20121028,'url':'http://www.sfgate.com/business/article/Solar-energy-is-ready-the-U-S-isn-t-3988796.php'};</v>
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s44 = {'publication':'SF Gate','date': 20121028,'url':'http://www.sfgate.com/business/article/Solar-energy-is-ready-the-U-S-isn-t-3988796.php',debate:'3'};</v>
       </c>
     </row>
     <row r="48" spans="1:7">

</xml_diff>

<commit_message>
Updated SF Gate info to contain Oct 29-Nov 5 data
</commit_message>
<xml_diff>
--- a/Newspapers.xlsx
+++ b/Newspapers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>Debate</t>
   </si>
@@ -181,6 +181,36 @@
   </si>
   <si>
     <t>http://www.sfgate.com/business/article/Solar-energy-is-ready-the-U-S-isn-t-3988796.php</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>29-Oct</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/opinion/openforum/article/Energy-debate-is-about-self-reliance-3991626.php</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/business/bloomberg/article/Obama-Tied-With-Romney-in-New-Polls-of-3994561.php</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/news/article/Obama-Romney-working-to-get-NH-voters-to-polls-3996943.php</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/business/prweb/article/Romney-is-Naughtier-than-Obama-says-4002000.php</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/opinion/article/Obama-Romney-stay-vague-on-foreign-policy-4004249.php</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/news/politics/article/At-the-end-Romney-Obama-spar-over-voter-revenge-4005194.php</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/news/politics/article/For-Romney-Obama-long-slog-to-nail-biter-finish-4006930.php</t>
+  </si>
+  <si>
+    <t>http://www.sfgate.com/news/politics/article/Obama-Romney-make-last-minute-pleas-in-close-race-4008287.php</t>
   </si>
 </sst>
 </file>
@@ -188,9 +218,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="164" formatCode="yyyymmdd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,16 +244,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -231,8 +275,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -350,19 +429,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="118">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -478,66 +563,250 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
         <right/>
-        <top/>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="yyyymmdd"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
-        <top/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thick">
+          <color theme="0"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -545,7 +814,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="yyyymmdd"/>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
@@ -556,13 +825,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G48" totalsRowCount="1">
-  <autoFilter ref="A3:G48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:G56" totalsRowCount="1">
+  <autoFilter ref="A3:G54"/>
   <tableColumns count="7">
     <tableColumn id="1" name="id" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Debate" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="Newspaper" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Date" dataDxfId="9" totalsRowDxfId="3"/>
+    <tableColumn id="2" name="Debate" totalsRowLabel="3" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Newspaper" totalsRowLabel="SF Gate" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Date" totalsRowLabel="29-Oct" dataDxfId="9" totalsRowDxfId="3"/>
     <tableColumn id="5" name="Formatted date" dataDxfId="8" totalsRowDxfId="2">
       <calculatedColumnFormula>D4</calculatedColumnFormula>
     </tableColumn>
@@ -897,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1254,7 +1523,7 @@
         <v>41191</v>
       </c>
       <c r="E15" s="3">
-        <f>D15</f>
+        <f t="shared" ref="E15:E52" si="1">D15</f>
         <v>41191</v>
       </c>
       <c r="F15" t="s">
@@ -1279,7 +1548,7 @@
         <v>41192</v>
       </c>
       <c r="E16" s="3">
-        <f>D16</f>
+        <f t="shared" si="1"/>
         <v>41192</v>
       </c>
       <c r="F16" t="s">
@@ -1304,7 +1573,7 @@
         <v>41193</v>
       </c>
       <c r="E17" s="3">
-        <f>D17</f>
+        <f t="shared" si="1"/>
         <v>41193</v>
       </c>
       <c r="F17" t="s">
@@ -1329,7 +1598,7 @@
         <v>41193</v>
       </c>
       <c r="E18" s="3">
-        <f>D18</f>
+        <f t="shared" si="1"/>
         <v>41193</v>
       </c>
       <c r="F18" t="s">
@@ -1354,7 +1623,7 @@
         <v>41194</v>
       </c>
       <c r="E19" s="3">
-        <f>D19</f>
+        <f t="shared" si="1"/>
         <v>41194</v>
       </c>
       <c r="F19" t="s">
@@ -1379,7 +1648,7 @@
         <v>41194</v>
       </c>
       <c r="E20" s="3">
-        <f>D20</f>
+        <f t="shared" si="1"/>
         <v>41194</v>
       </c>
       <c r="F20" t="s">
@@ -1404,7 +1673,7 @@
         <v>41195</v>
       </c>
       <c r="E21" s="3">
-        <f>D21</f>
+        <f t="shared" si="1"/>
         <v>41195</v>
       </c>
       <c r="F21" t="s">
@@ -1429,7 +1698,7 @@
         <v>41196</v>
       </c>
       <c r="E22" s="3">
-        <f>D22</f>
+        <f t="shared" si="1"/>
         <v>41196</v>
       </c>
       <c r="F22" t="s">
@@ -1454,7 +1723,7 @@
         <v>41197</v>
       </c>
       <c r="E23" s="3">
-        <f>D23</f>
+        <f t="shared" si="1"/>
         <v>41197</v>
       </c>
       <c r="F23" t="s">
@@ -1479,7 +1748,7 @@
         <v>41197</v>
       </c>
       <c r="E24" s="3">
-        <f>D24</f>
+        <f t="shared" si="1"/>
         <v>41197</v>
       </c>
       <c r="F24" t="s">
@@ -1504,7 +1773,7 @@
         <v>41198</v>
       </c>
       <c r="E25" s="3">
-        <f>D25</f>
+        <f t="shared" si="1"/>
         <v>41198</v>
       </c>
       <c r="F25" t="s">
@@ -1529,7 +1798,7 @@
         <v>41198</v>
       </c>
       <c r="E26" s="3">
-        <f>D26</f>
+        <f t="shared" si="1"/>
         <v>41198</v>
       </c>
       <c r="F26" t="s">
@@ -1554,7 +1823,7 @@
         <v>41198</v>
       </c>
       <c r="E27" s="7">
-        <f>D27</f>
+        <f t="shared" si="1"/>
         <v>41198</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -1579,7 +1848,7 @@
         <v>41199</v>
       </c>
       <c r="E28" s="7">
-        <f>D28</f>
+        <f t="shared" si="1"/>
         <v>41199</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -1604,7 +1873,7 @@
         <v>41199</v>
       </c>
       <c r="E29" s="7">
-        <f>D29</f>
+        <f t="shared" si="1"/>
         <v>41199</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -1629,7 +1898,7 @@
         <v>41200</v>
       </c>
       <c r="E30" s="7">
-        <f>D30</f>
+        <f t="shared" si="1"/>
         <v>41200</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1654,7 +1923,7 @@
         <v>41200</v>
       </c>
       <c r="E31" s="7">
-        <f>D31</f>
+        <f t="shared" si="1"/>
         <v>41200</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -1679,7 +1948,7 @@
         <v>41200</v>
       </c>
       <c r="E32" s="7">
-        <f>D32</f>
+        <f t="shared" si="1"/>
         <v>41200</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -1704,7 +1973,7 @@
         <v>41201</v>
       </c>
       <c r="E33" s="7">
-        <f>D33</f>
+        <f t="shared" si="1"/>
         <v>41201</v>
       </c>
       <c r="F33" s="5" t="s">
@@ -1729,7 +1998,7 @@
         <v>41201</v>
       </c>
       <c r="E34" s="7">
-        <f>D34</f>
+        <f t="shared" si="1"/>
         <v>41201</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -1754,7 +2023,7 @@
         <v>41202</v>
       </c>
       <c r="E35" s="7">
-        <f>D35</f>
+        <f t="shared" si="1"/>
         <v>41202</v>
       </c>
       <c r="F35" s="5" t="s">
@@ -1779,7 +2048,7 @@
         <v>41202</v>
       </c>
       <c r="E36" s="7">
-        <f>D36</f>
+        <f t="shared" si="1"/>
         <v>41202</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -1804,7 +2073,7 @@
         <v>41203</v>
       </c>
       <c r="E37" s="7">
-        <f>D37</f>
+        <f t="shared" si="1"/>
         <v>41203</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -1829,7 +2098,7 @@
         <v>41203</v>
       </c>
       <c r="E38" s="7">
-        <f>D38</f>
+        <f t="shared" si="1"/>
         <v>41203</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -1854,7 +2123,7 @@
         <v>41204</v>
       </c>
       <c r="E39" s="7">
-        <f>D39</f>
+        <f t="shared" si="1"/>
         <v>41204</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -1879,7 +2148,7 @@
         <v>41204</v>
       </c>
       <c r="E40" s="7">
-        <f>D40</f>
+        <f t="shared" si="1"/>
         <v>41204</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -1904,7 +2173,7 @@
         <v>41205</v>
       </c>
       <c r="E41" s="7">
-        <f>D41</f>
+        <f t="shared" si="1"/>
         <v>41205</v>
       </c>
       <c r="F41" s="5" t="s">
@@ -1929,7 +2198,7 @@
         <v>41205</v>
       </c>
       <c r="E42" s="7">
-        <f>D42</f>
+        <f t="shared" si="1"/>
         <v>41205</v>
       </c>
       <c r="F42" s="5" t="s">
@@ -1954,7 +2223,7 @@
         <v>41206</v>
       </c>
       <c r="E43" s="7">
-        <f>D43</f>
+        <f t="shared" si="1"/>
         <v>41206</v>
       </c>
       <c r="F43" s="5" t="s">
@@ -1979,7 +2248,7 @@
         <v>41207</v>
       </c>
       <c r="E44" s="7">
-        <f>D44</f>
+        <f t="shared" si="1"/>
         <v>41207</v>
       </c>
       <c r="F44" s="5" t="s">
@@ -2004,7 +2273,7 @@
         <v>41208</v>
       </c>
       <c r="E45" s="7">
-        <f>D45</f>
+        <f t="shared" si="1"/>
         <v>41208</v>
       </c>
       <c r="F45" s="5" t="s">
@@ -2029,7 +2298,7 @@
         <v>41209</v>
       </c>
       <c r="E46" s="7">
-        <f>D46</f>
+        <f t="shared" si="1"/>
         <v>41209</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -2054,7 +2323,7 @@
         <v>41210</v>
       </c>
       <c r="E47" s="7">
-        <f>D47</f>
+        <f t="shared" si="1"/>
         <v>41210</v>
       </c>
       <c r="F47" s="5" t="s">
@@ -2066,13 +2335,219 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="8"/>
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="4">
+        <v>41211</v>
+      </c>
+      <c r="E48" s="7">
+        <f t="shared" si="1"/>
+        <v>41211</v>
+      </c>
+      <c r="F48" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s45 = {'publication':'SF Gate','date': 20121029,'url':'http://www.sfgate.com/opinion/openforum/article/Energy-debate-is-about-self-reliance-3991626.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="4">
+        <v>41212</v>
+      </c>
+      <c r="E49" s="7">
+        <f t="shared" si="1"/>
+        <v>41212</v>
+      </c>
+      <c r="F49" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s46 = {'publication':'SF Gate','date': 20121030,'url':'http://www.sfgate.com/business/bloomberg/article/Obama-Tied-With-Romney-in-New-Polls-of-3994561.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="4">
+        <v>41213</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="1"/>
+        <v>41213</v>
+      </c>
+      <c r="F50" t="s">
+        <v>58</v>
+      </c>
+      <c r="G50" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s47 = {'publication':'SF Gate','date': 20121031,'url':'http://www.sfgate.com/news/article/Obama-Romney-working-to-get-NH-voters-to-polls-3996943.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="4">
+        <v>41214</v>
+      </c>
+      <c r="E51" s="7">
+        <f t="shared" si="1"/>
+        <v>41214</v>
+      </c>
+      <c r="F51" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s48 = {'publication':'SF Gate','date': 20121101,'url':'http://www.sfgate.com/business/prweb/article/Romney-is-Naughtier-than-Obama-says-4002000.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="4">
+        <v>41215</v>
+      </c>
+      <c r="E52" s="7">
+        <f t="shared" si="1"/>
+        <v>41215</v>
+      </c>
+      <c r="F52" t="s">
+        <v>60</v>
+      </c>
+      <c r="G52" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s49 = {'publication':'SF Gate','date': 20121102,'url':'http://www.sfgate.com/opinion/article/Obama-Romney-stay-vague-on-foreign-policy-4004249.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="4">
+        <v>41216</v>
+      </c>
+      <c r="E53" s="3">
+        <f>D53</f>
+        <v>41216</v>
+      </c>
+      <c r="F53" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s50 = {'publication':'SF Gate','date': 20121103,'url':'http://www.sfgate.com/news/politics/article/At-the-end-Romney-Obama-spar-over-voter-revenge-4005194.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="4">
+        <v>41217</v>
+      </c>
+      <c r="E54" s="3">
+        <f>D54</f>
+        <v>41217</v>
+      </c>
+      <c r="F54" t="s">
+        <v>62</v>
+      </c>
+      <c r="G54" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s51 = {'publication':'SF Gate','date': 20121104,'url':'http://www.sfgate.com/news/politics/article/For-Romney-Obama-long-slog-to-nail-biter-finish-4006930.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="16" thickBot="1">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="4">
+        <v>41218</v>
+      </c>
+      <c r="E55" s="3">
+        <f>D55</f>
+        <v>41218</v>
+      </c>
+      <c r="F55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G55" s="13" t="str">
+        <f>CONCATENATE("var s",Table1[[#This Row],[id]]," = {'publication':'",Table1[[#This Row],[Newspaper]],"','date': ",TEXT(Table1[[#This Row],[Formatted date]],"yyyymmdd"),",'url':'",Table1[[#This Row],[URL]],"',debate:'",Table1[[#This Row],[Debate]],"'};")</f>
+        <v>var s52 = {'publication':'SF Gate','date': 20121105,'url':'http://www.sfgate.com/news/politics/article/Obama-Romney-make-last-minute-pleas-in-close-race-4008287.php',debate:'3'};</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="16" thickTop="1">
+      <c r="A56" s="9"/>
+      <c r="B56" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updates to readme and to API python scripts and moved unused documents to 'Unused' folder
</commit_message>
<xml_diff>
--- a/Newspapers.xlsx
+++ b/Newspapers.xlsx
@@ -311,9 +311,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="118">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -447,7 +448,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="118">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -564,6 +565,7 @@
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1168,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>